<commit_message>
Control powerflow with constant values
</commit_message>
<xml_diff>
--- a/Mini-projet-trey_Buchser_Joye/data/trey_power_network.xlsx
+++ b/Mini-projet-trey_Buchser_Joye/data/trey_power_network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\matthjoye\github\rhtlab_MIB\Mini-projet-trey_Buchser_Joye\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594ACC54-A1A8-4269-8422-C996EC8905D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DCE557-250A-4A59-BA8B-E49656DFEDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="5520" yWindow="3192" windowWidth="11580" windowHeight="8856" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -2578,7 +2578,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2637,6 +2637,9 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2648,6 +2651,9 @@
       <c r="C3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -2659,6 +2665,9 @@
       <c r="C4">
         <v>2</v>
       </c>
+      <c r="D4">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -2670,6 +2679,9 @@
       <c r="C5">
         <v>3</v>
       </c>
+      <c r="D5">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -2681,6 +2693,9 @@
       <c r="C6">
         <v>4</v>
       </c>
+      <c r="D6">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -2692,6 +2707,9 @@
       <c r="C7">
         <v>5</v>
       </c>
+      <c r="D7">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -2703,6 +2721,9 @@
       <c r="C8">
         <v>6</v>
       </c>
+      <c r="D8">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -2714,6 +2735,9 @@
       <c r="C9">
         <v>7</v>
       </c>
+      <c r="D9">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -2725,6 +2749,9 @@
       <c r="C10">
         <v>8</v>
       </c>
+      <c r="D10">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -2736,6 +2763,9 @@
       <c r="C11">
         <v>9</v>
       </c>
+      <c r="D11">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -2747,6 +2777,9 @@
       <c r="C12">
         <v>10</v>
       </c>
+      <c r="D12">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -2757,6 +2790,9 @@
       </c>
       <c r="C13">
         <v>11</v>
+      </c>
+      <c r="D13">
+        <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Commit before testing trey_power_network overwritting
</commit_message>
<xml_diff>
--- a/Mini-projet-trey_Buchser_Joye/data/trey_power_network.xlsx
+++ b/Mini-projet-trey_Buchser_Joye/data/trey_power_network.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micael\git\rhtlab_MIB\Mini-projet-trey_Buchser_Joye\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB794B0-F22E-44EC-8244-D067C535510E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6084A5A5-08AD-4EC2-9877-9BB17C65B7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
@@ -2575,10 +2575,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AA0C-6E10-4C2C-B831-A2E20673E5F8}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2696,9 +2696,6 @@
       <c r="D6">
         <v>0.01</v>
       </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -2727,9 +2724,6 @@
       <c r="D8">
         <v>0.01</v>
       </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -2744,9 +2738,6 @@
       <c r="D9">
         <v>0.01</v>
       </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -2775,9 +2766,6 @@
       <c r="D11">
         <v>0.01</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -2805,101 +2793,6 @@
       </c>
       <c r="D13">
         <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>